<commit_message>
-> Scripting DPLKINV134-001,DPLKINV134-002 (Approve Ticket) -> Scripting DPLKINV136-001,DPLKINV136-002 (Approve Switching) -> Scripting DPLKINV157-001 until DPLKINV159-002 (Subscr and Deviden)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS141-001 - Kepesertaan - Proses - Reverse Deposit(Bulk).xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS141-001 - Kepesertaan - Proses - Reverse Deposit(Bulk).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8372C0-94ED-4B36-A0F8-18469007CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6491E38-6584-4F5D-AA80-0AB637FA6C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653A54F0-D01B-49C0-BB41-F0FC7D2164BA}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>